<commit_message>
Completed 1.1 and 1.2
</commit_message>
<xml_diff>
--- a/SP500/11/Results.xlsx
+++ b/SP500/11/Results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="11">
   <si>
     <t xml:space="preserve">Function</t>
   </si>
@@ -44,6 +44,15 @@
   </si>
   <si>
     <t xml:space="preserve">sigmoid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">leaky</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 components</t>
   </si>
 </sst>
 </file>
@@ -58,6 +67,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -149,17 +159,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.5867346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -349,20 +359,20 @@
         <v>0.000253</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+    <row r="12" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="1" t="n">
         <v>0.1</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C12" s="1" t="n">
         <v>0.000248</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="D12" s="1" t="n">
         <v>0.000258</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="E12" s="1" t="n">
         <v>0.000252</v>
       </c>
     </row>
@@ -432,6 +442,102 @@
       </c>
       <c r="E16" s="0" t="n">
         <v>0.188696</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>0.000282</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>0.050595</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>0.010952</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>0.000223</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>0.00025</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>0.000233</v>
+      </c>
+    </row>
+    <row r="19" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="1" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <v>0.000189</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>0.000231</v>
+      </c>
+      <c r="E19" s="1" t="n">
+        <v>0.000224</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>0.000238</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>0.000241</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>0.00024</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>1E-005</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>0.000268</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>0.000272</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>0.00027</v>
+      </c>
+    </row>
+    <row r="22" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="1" t="n">
+        <v>0.000142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>